<commit_message>
added another entry in logbook about the function get_priority()
</commit_message>
<xml_diff>
--- a/CS342Logbook.xlsx
+++ b/CS342Logbook.xlsx
@@ -124,7 +124,7 @@
     <t xml:space="preserve">thread.c</t>
   </si>
   <si>
-    <t xml:space="preserve">thread_set_priority() </t>
+    <t xml:space="preserve">thread_set_priority() thread_get_priority() </t>
   </si>
   <si>
     <t xml:space="preserve">16 of 50 tests still FAIL</t>
@@ -279,26 +279,26 @@
   <dimension ref="A1:Q5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+      <selection pane="topLeft" activeCell="I6" activeCellId="0" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.63967611336032"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.5668016194332"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.74898785425101"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.6761133603239"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.3562753036437"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.6396761133603"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="9.63967611336032"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.748987854251"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="9.74898785425101"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.31983805668016"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.4615384615385"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.5668016194332"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.6761133603239"/>
     <col collapsed="false" hidden="false" max="10" min="9" style="0" width="13.7125506072874"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="15.4251012145749"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="15.2105263157895"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="15.5303643724696"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="15.3198380566802"/>
     <col collapsed="false" hidden="false" max="13" min="13" style="0" width="10.6032388663968"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="12.4251012145749"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="12.5344129554656"/>
     <col collapsed="false" hidden="false" max="15" min="15" style="0" width="11.3562753036437"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="15.6396761133603"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="15.7449392712551"/>
     <col collapsed="false" hidden="false" max="17" min="17" style="0" width="14.1417004048583"/>
     <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="8.57085020242915"/>
   </cols>

</xml_diff>

<commit_message>
UP02 with logbook updated
</commit_message>
<xml_diff>
--- a/CS342Logbook.xlsx
+++ b/CS342Logbook.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="112">
   <si>
     <t>Session</t>
   </si>
@@ -331,13 +331,22 @@
     <t>pagefault()</t>
   </si>
   <si>
-    <t>29</t>
+    <t>36</t>
   </si>
   <si>
     <t>40 of 76 tests fail</t>
   </si>
   <si>
     <t>Interrupts and system calls</t>
+  </si>
+  <si>
+    <t>5 mins</t>
+  </si>
+  <si>
+    <t>Logbook updated</t>
+  </si>
+  <si>
+    <t>UP02 with logbook updated</t>
   </si>
 </sst>
 </file>
@@ -2657,23 +2666,47 @@
       <c r="AB18" s="4"/>
     </row>
     <row r="19" ht="15" customHeight="1">
-      <c r="A19" s="4"/>
-      <c r="B19" s="11"/>
-      <c r="C19" s="9"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
-      <c r="H19" s="4"/>
-      <c r="I19" s="4"/>
-      <c r="J19" s="4"/>
-      <c r="K19" s="4"/>
-      <c r="L19" s="4"/>
-      <c r="M19" s="8"/>
-      <c r="N19" s="4"/>
-      <c r="O19" s="4"/>
-      <c r="P19" s="4"/>
-      <c r="Q19" s="4"/>
+      <c r="A19" t="s" s="4">
+        <v>33</v>
+      </c>
+      <c r="B19" s="11">
+        <v>43018</v>
+      </c>
+      <c r="C19" s="9">
+        <v>43018.020833333336</v>
+      </c>
+      <c r="D19" t="s" s="4">
+        <v>19</v>
+      </c>
+      <c r="E19" t="s" s="4">
+        <v>109</v>
+      </c>
+      <c r="F19" t="s" s="4">
+        <v>91</v>
+      </c>
+      <c r="G19" t="s" s="4">
+        <v>110</v>
+      </c>
+      <c r="H19" s="8"/>
+      <c r="I19" s="8"/>
+      <c r="J19" s="8"/>
+      <c r="K19" s="8"/>
+      <c r="L19" s="8"/>
+      <c r="M19" s="10">
+        <v>0</v>
+      </c>
+      <c r="N19" t="s" s="4">
+        <v>100</v>
+      </c>
+      <c r="O19" t="s" s="4">
+        <v>106</v>
+      </c>
+      <c r="P19" t="s" s="4">
+        <v>107</v>
+      </c>
+      <c r="Q19" t="s" s="4">
+        <v>111</v>
+      </c>
       <c r="R19" s="4"/>
       <c r="S19" s="4"/>
       <c r="T19" s="4"/>
@@ -2717,12 +2750,13 @@
       <c r="AB20" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
+    <mergeCell ref="G19:L19"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="G12:Q12"/>
+    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="J1:L1"/>
     <mergeCell ref="M1:Q1"/>
-    <mergeCell ref="J1:L1"/>
-    <mergeCell ref="G1:I1"/>
-    <mergeCell ref="G12:Q12"/>
-    <mergeCell ref="A1:F1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511806" footer="0.511806"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>

</xml_diff>